<commit_message>
Poista Excel-puolen validointi päivämääräkentästä
</commit_message>
<xml_diff>
--- a/dev-resources/excel/harja_reikapaikkausten_pohja.xlsx
+++ b/dev-resources/excel/harja_reikapaikkausten_pohja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panu.pasanen/Downloads/excelpohjauusinpulla/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panu.pasanen/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959B8DB5-EFEC-914D-A002-B09C05C4D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA142DFB-200D-5740-A1D0-B9DF5118E200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40020" yWindow="500" windowWidth="30760" windowHeight="28300" xr2:uid="{59B07E82-4145-2244-B2B8-7A6E24D805F3}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{59B07E82-4145-2244-B2B8-7A6E24D805F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Tätä exceliä ei ole tarkoitettu ohjelmoitujen paikkausten tietojen tuontiin. Näitä varten on Harjassa sivu "Muut paikkaukset" → "Paikkauskohteet"</t>
+      <t>Tämä excel on tarkoitettu kohteettomien reikäpaikkausten tietojen tuontiin. Muita paikkauksia varten harjassa on välilehti "Muut paikkaukset" → "Paikkauskohteet"</t>
     </r>
   </si>
 </sst>
@@ -801,7 +801,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,13 +899,10 @@
       <c r="F20" s="22"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Virheellinen tunniste" error="Tunnisteen tulee olla numeerinen arvo." sqref="A4:A1048576" xr:uid="{E55D10B6-8E53-AF48-9EEE-E72A5611D938}">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Virheellinen syöte" error="Tiedon tulee olla validi päivämäärä (xx.xx.xxxx)" sqref="B4:B1048576" xr:uid="{A9C431C6-75E5-B54C-A918-FD1103970469}">
-      <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Virheellinen syöte" error="Tiedon tulee olla numeerinen arvo." sqref="I4:I1048576 K4:K1048576" xr:uid="{30F6D3A9-A2FE-904B-8C30-B1B3962D8419}">
       <formula1>0</formula1>

</xml_diff>

<commit_message>
Päivitä reikäpaikkausten pohja- excel (poista pvm validointi)
</commit_message>
<xml_diff>
--- a/dev-resources/excel/harja_reikapaikkausten_pohja.xlsx
+++ b/dev-resources/excel/harja_reikapaikkausten_pohja.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panu.pasanen/Downloads/excelpohjauusinpulla/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panu.pasanen/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959B8DB5-EFEC-914D-A002-B09C05C4D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA142DFB-200D-5740-A1D0-B9DF5118E200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40020" yWindow="500" windowWidth="30760" windowHeight="28300" xr2:uid="{59B07E82-4145-2244-B2B8-7A6E24D805F3}"/>
+    <workbookView xWindow="-30240" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{59B07E82-4145-2244-B2B8-7A6E24D805F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Tätä exceliä ei ole tarkoitettu ohjelmoitujen paikkausten tietojen tuontiin. Näitä varten on Harjassa sivu "Muut paikkaukset" → "Paikkauskohteet"</t>
+      <t>Tämä excel on tarkoitettu kohteettomien reikäpaikkausten tietojen tuontiin. Muita paikkauksia varten harjassa on välilehti "Muut paikkaukset" → "Paikkauskohteet"</t>
     </r>
   </si>
 </sst>
@@ -801,7 +801,7 @@
   <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,13 +899,10 @@
       <c r="F20" s="22"/>
     </row>
   </sheetData>
-  <dataValidations count="4">
+  <dataValidations count="3">
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" errorTitle="Virheellinen tunniste" error="Tunnisteen tulee olla numeerinen arvo." sqref="A4:A1048576" xr:uid="{E55D10B6-8E53-AF48-9EEE-E72A5611D938}">
       <formula1>0</formula1>
       <formula2>1000000000</formula2>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Virheellinen syöte" error="Tiedon tulee olla validi päivämäärä (xx.xx.xxxx)" sqref="B4:B1048576" xr:uid="{A9C431C6-75E5-B54C-A918-FD1103970469}">
-      <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Virheellinen syöte" error="Tiedon tulee olla numeerinen arvo." sqref="I4:I1048576 K4:K1048576" xr:uid="{30F6D3A9-A2FE-904B-8C30-B1B3962D8419}">
       <formula1>0</formula1>

</xml_diff>